<commit_message>
21 September Push All pages
</commit_message>
<xml_diff>
--- a/public/academics_excel/pg_semester1.xlsx
+++ b/public/academics_excel/pg_semester1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_page\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\s417\dept_website\public\academics_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{096608D3-5E52-49F2-9BFE-02D5CFD487C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123D7A7D-3A8A-49F8-A99A-16EA38EC2CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E455C53A-8806-482C-976B-55432FEC1D96}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{E455C53A-8806-482C-976B-55432FEC1D96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>CourseNo</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>SEM-1</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -461,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7371BF44-7030-4579-8D37-803196F29715}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,14 +567,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>